<commit_message>
Fix column name for POL, POD (6->5) in convert script Fix column name TEMP. (C) -> TEMP. ('C) for excel templates
</commit_message>
<xml_diff>
--- a/app/static/xls_template/DischList_Template.xlsx
+++ b/app/static/xls_template/DischList_Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyProject\Flask_web\app\xls_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyProject\EDI_APP_TEST\app\static\xls_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E524F2B0-E21B-4CD5-8FDC-9E31E5B8A104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79CA20E-B9E6-4B9E-9AD4-57DDBCF49A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7F5E6C24-73B4-4E8B-A3E7-24E78EE6A89A}"/>
   </bookViews>
@@ -47,12 +47,6 @@
   </si>
   <si>
     <t>OPS (3 LETTERS)</t>
-  </si>
-  <si>
-    <t>POL (6 LETTERS)</t>
-  </si>
-  <si>
-    <t>POD (6 LETTERS)</t>
   </si>
   <si>
     <t>FPOD (IF ANY)</t>
@@ -119,6 +113,12 @@
   </si>
   <si>
     <t>SEAL4</t>
+  </si>
+  <si>
+    <t>POL (5 LETTERS)</t>
+  </si>
+  <si>
+    <t>POD (5 LETTERS)</t>
   </si>
 </sst>
 </file>
@@ -989,8 +989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB36EFB-5200-432B-9E6C-BC6C2EDF13CB}">
   <dimension ref="A1:AG159"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1037,16 +1037,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>30</v>
-      </c>
-      <c r="F1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" t="s">
-        <v>32</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -1067,64 +1067,64 @@
         <v>8</v>
       </c>
       <c r="N1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>17</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>26</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">

</xml_diff>